<commit_message>
getting lab 3 and challenge 3 up.
</commit_message>
<xml_diff>
--- a/00-course-info/course-schedule.xlsx
+++ b/00-course-info/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/erobin17_calpoly_edu/Documents/stat-331-calpoly/00-course-info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="996" documentId="11_F25DC773A252ABDACC1048BFF9586A525BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F796DFC7-161F-4B88-98D5-7E1CD33ED357}"/>
+  <xr:revisionPtr revIDLastSave="1009" documentId="11_F25DC773A252ABDACC1048BFF9586A525BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97EADDE2-6CAD-4AA6-A91B-4C310D43FAEB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="188">
   <si>
     <t>Week</t>
   </si>
@@ -644,9 +644,6 @@
     <t>Lab3: Murder in SQL City</t>
   </si>
   <si>
-    <t>Lab2: Data Frames (Video Games)</t>
-  </si>
-  <si>
     <t>PA: Identify the mystery college</t>
   </si>
   <si>
@@ -671,23 +668,35 @@
     <t>Data Structures: Review Vecrors/Matrices/etc.</t>
   </si>
   <si>
-    <t>Concept Check: Prereading Quiz</t>
-  </si>
-  <si>
     <t>Tidy Data + Basics of Data Visualization (ggplot)</t>
   </si>
   <si>
-    <t>Lab1: Intro to Quarto (incorporate spiral + madlibs + fizzbuzz?)</t>
-  </si>
-  <si>
     <t>Midterm Exam???</t>
+  </si>
+  <si>
+    <t>PA 1: Find the mistakes (poem)</t>
+  </si>
+  <si>
+    <t>PA 2: Using Data Visualization to Find the Penguins</t>
+  </si>
+  <si>
+    <t>Lab2: Exploring Rodents with ggplot2</t>
+  </si>
+  <si>
+    <t>Challenge: Spicing things up with ggplot2</t>
+  </si>
+  <si>
+    <t>Lab1: Intro to Quarto</t>
+  </si>
+  <si>
+    <t>FizzBuzz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,6 +750,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -787,7 +803,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -831,6 +847,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1118,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1128,7 +1145,7 @@
     <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.88671875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="5" max="5" width="61.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.44140625" customWidth="1"/>
     <col min="7" max="7" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="69.6640625" bestFit="1" customWidth="1"/>
@@ -1229,7 +1246,7 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="D3" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>164</v>
@@ -1260,11 +1277,11 @@
         <v>6</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="16" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>88</v>
@@ -1286,10 +1303,10 @@
         <v>68</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>154</v>
@@ -1309,10 +1326,10 @@
         <v>8</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>86</v>
+        <v>183</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>166</v>
@@ -1364,8 +1381,8 @@
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="22" t="s">
-        <v>163</v>
+      <c r="F8" s="9" t="s">
+        <v>184</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>136</v>
@@ -1377,7 +1394,7 @@
         <v>14</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N8" t="s">
         <v>114</v>
@@ -1387,8 +1404,8 @@
       <c r="B9" s="5"/>
       <c r="C9" s="8"/>
       <c r="E9" s="21"/>
-      <c r="F9" s="21" t="s">
-        <v>172</v>
+      <c r="F9" s="27" t="s">
+        <v>185</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>157</v>
@@ -1408,7 +1425,7 @@
         <v>168</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>56</v>
@@ -1431,9 +1448,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
-      <c r="E11" s="9" t="s">
-        <v>149</v>
-      </c>
+      <c r="E11" s="9"/>
       <c r="G11" s="9" t="s">
         <v>138</v>
       </c>
@@ -1503,7 +1518,7 @@
         <v>98</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>57</v>
@@ -1584,7 +1599,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>138</v>
@@ -1608,7 +1623,7 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="E19" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="9" t="s">
@@ -1630,7 +1645,7 @@
       </c>
       <c r="E20" s="23"/>
       <c r="F20" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>101</v>
@@ -1713,7 +1728,7 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>103</v>
@@ -1965,7 +1980,7 @@
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>151</v>
@@ -2069,14 +2084,12 @@
     <hyperlink ref="J19" r:id="rId21" xr:uid="{0B04BF78-9EE4-43BF-82F6-B581BC24146C}"/>
     <hyperlink ref="J21" r:id="rId22" xr:uid="{44A13C4E-7496-4A3D-9945-E628ABF4F337}"/>
     <hyperlink ref="J23" r:id="rId23" xr:uid="{CE13A70E-CC36-4ADC-9A3E-580BA2EDED19}"/>
-    <hyperlink ref="F9" r:id="rId24" display="HW6: Data Frames (Video Games)" xr:uid="{2E3412C8-2BBA-4A6A-B162-F38F23598A8F}"/>
-    <hyperlink ref="F13" r:id="rId25" display="HW8: Murder in SQL City" xr:uid="{65C178E5-D1E2-4A2C-B6B2-53A4DF52F2DC}"/>
-    <hyperlink ref="F8" r:id="rId26" xr:uid="{9B3A5166-9122-4506-97D8-56D10A3D5384}"/>
-    <hyperlink ref="E30" r:id="rId27" xr:uid="{7384CE21-0B83-44EF-A91A-B6EBBFADD5FF}"/>
+    <hyperlink ref="F13" r:id="rId24" display="HW8: Murder in SQL City" xr:uid="{65C178E5-D1E2-4A2C-B6B2-53A4DF52F2DC}"/>
+    <hyperlink ref="E30" r:id="rId25" xr:uid="{7384CE21-0B83-44EF-A91A-B6EBBFADD5FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
-  <legacyDrawing r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
+  <legacyDrawing r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
adjusted points for challenge
</commit_message>
<xml_diff>
--- a/00-course-info/course-schedule.xlsx
+++ b/00-course-info/course-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/erobin17_calpoly_edu/Documents/stat-331-calpoly/00-course-info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1148" documentId="11_F25DC773A252ABDACC1048BFF9586A525BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E23AB33-E5DD-4FCF-9A03-DBF049820828}"/>
+  <xr:revisionPtr revIDLastSave="1149" documentId="11_F25DC773A252ABDACC1048BFF9586A525BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F28E86A-2229-4D21-BF14-326CB8C52B86}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -731,13 +731,13 @@
     <t>Lab7: Functions &amp; Fish</t>
   </si>
   <si>
-    <t>Bonus Challenge: Data Mishaps Night (+10)</t>
-  </si>
-  <si>
     <t>Challenge: Incorporating Multiple Inputs (+10)</t>
   </si>
   <si>
     <t>No Challenge this week</t>
+  </si>
+  <si>
+    <t>Bonus Challenge: Data Mishaps Night (+8)</t>
   </si>
 </sst>
 </file>
@@ -1202,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>101</v>
@@ -1911,7 +1911,7 @@
       <c r="B29" s="1"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -1929,7 +1929,7 @@
       <c r="B31" s="1"/>
       <c r="E31" s="9"/>
       <c r="F31" s="27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>

</xml_diff>